<commit_message>
fix: add more and fix bugs
</commit_message>
<xml_diff>
--- a/14.paintballres/extracted_data/14.Data.xlsx
+++ b/14.paintballres/extracted_data/14.Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="302">
   <si>
     <t>location_name</t>
   </si>
@@ -23,6 +23,9 @@
     <t>address</t>
   </si>
   <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
     <t>imgLink</t>
   </si>
   <si>
@@ -38,6 +41,9 @@
     <t>Hialeah, FL  33014</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>https://paintballreservations.com/action_town_paintball_field/detail_page_images/ActionTown/Logo2%20smaller.png</t>
   </si>
   <si>
@@ -101,6 +107,9 @@
     <t>Code Red Mobile Laser Tag is a company that provides laser tag events at your location.  For information and reservations, call them directly at (972) 834-0733.  Visit their website at www.coderedlasertag.com</t>
   </si>
   <si>
+    <t>(972) 834-0733</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/code_red_mobile_laser_tag/detail_page_images/CodeRed/</t>
   </si>
   <si>
@@ -116,7 +125,7 @@
     <t>Collin County</t>
   </si>
   <si>
-    <t>https://paintballreservations.com/collin_county_paintball/detail_page_images/CollinCounty/</t>
+    <t>http://paintballreservations.com/collin_county_paintball/detail_page_images/CollinCounty/</t>
   </si>
   <si>
     <t>Combat Zone Paintball - Las Vegas</t>
@@ -143,6 +152,9 @@
     <t>Yolo County</t>
   </si>
   <si>
+    <t>(530) 757-7700</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/davis_paintball_center/detail_page_images/davis/logo.jpg</t>
   </si>
   <si>
@@ -158,6 +170,9 @@
     <t>Denton County</t>
   </si>
   <si>
+    <t>(817) 854-0085</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/dfw_adventure_park/detail_page_images/DFWAdventure/</t>
   </si>
   <si>
@@ -173,6 +188,9 @@
     <t>Johnson County</t>
   </si>
   <si>
+    <t>(817) 790-3831</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/dfw_pro_paintball_park/detail_page_images/DFWPaintball/</t>
   </si>
   <si>
@@ -203,12 +221,18 @@
     <t>Snohomish County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/eastside_airsoft/detail_page_images/eastside-airsoft/espb%20facebook%20logo%203.gif</t>
+    <t>(425) 780-5515</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/eastside_airsoft/detail_page_images/eastside-airsoft/espb%20facebook%20logo%203.gif</t>
   </si>
   <si>
     <t>21001 lake fontal rd</t>
   </si>
   <si>
+    <t>(425) 440-0845</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/eastside_paintball/detail_page_images/eastside/EastsideBanner.jpg</t>
   </si>
   <si>
@@ -218,7 +242,10 @@
     <t>16320 High Bridge Rd</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/eastside_zombie/detail_page_images/eastside-zombie/</t>
+    <t>(425) 939-8574</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/eastside_zombie/detail_page_images/eastside-zombie/</t>
   </si>
   <si>
     <t>Ellen's Amusement Center</t>
@@ -233,7 +260,10 @@
     <t>Dallas County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/ellen_amusement_center/detail_page_images/EllenAmusement/</t>
+    <t>(972) 291-4242</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/ellen_amusement_center/detail_page_images/EllenAmusement/</t>
   </si>
   <si>
     <t>20 S Union RD</t>
@@ -245,7 +275,7 @@
     <t>Grays Harbor County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/elma_paintball/detail_page_images/ElmaPaintball/468x92%202.jpg</t>
+    <t>https://paintballreservations.com/elma_paintball/detail_page_images/ElmaPaintball/468x92%202.jpg</t>
   </si>
   <si>
     <t>Extreme Rage Paintball Park</t>
@@ -272,6 +302,9 @@
     <t>Fun on the Run Paintball Park is the oldest and biggest paintball field in Fort Worth, Texas.  For information and reservations, call them directly at  (817) 237-0299.  Their web address is www.paintballfunontherun.com</t>
   </si>
   <si>
+    <t>(817) 237-0299</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/fun_on_the_run_paintball/detail_page_images/FunRun/</t>
   </si>
   <si>
@@ -287,6 +320,9 @@
     <t>Gatsplat is the only indoor paintball field in the Dallas-Fort Worth area.  For information and reservations, call them directly at (972) 956-5500.  Their web address is www.gatsplat.com/</t>
   </si>
   <si>
+    <t>(972) 956-5500</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/gat_splat_indoor_paintball_field/detail_page_images/Gatsplat/</t>
   </si>
   <si>
@@ -302,6 +338,9 @@
     <t>Whatcom County</t>
   </si>
   <si>
+    <t>(866) 784-5100</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/go_big_paintball_park/detail_page_images/gobig/</t>
   </si>
   <si>
@@ -416,6 +455,9 @@
     <t>Mason County</t>
   </si>
   <si>
+    <t>(360) 277-9369</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/master_blasters_paintball/detail_page_images/master-blasters/</t>
   </si>
   <si>
@@ -458,6 +500,9 @@
     <t>Arlington, WA  98223</t>
   </si>
   <si>
+    <t>(360) 799-5431</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/monkey_time_paintball_airsoft/detail_page_images/monkey-time/Banner.jpg</t>
   </si>
   <si>
@@ -467,6 +512,9 @@
     <t>19677 State Route 2</t>
   </si>
   <si>
+    <t>(360) 836-4846</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/monroe_paintball/detail_page_images/monroe-paintball/</t>
   </si>
   <si>
@@ -482,6 +530,9 @@
     <t>Skagit County</t>
   </si>
   <si>
+    <t>(360) 504-9452</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/mount_vernon_paintball_field/detail_page_images/mt-vernon/</t>
   </si>
   <si>
@@ -497,7 +548,10 @@
     <t>Cecil County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/north_east_adventure/detail_page_images/Northeast/</t>
+    <t>(410) 287-5227</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/north_east_adventure/detail_page_images/Northeast/</t>
   </si>
   <si>
     <t>Off The Wall Adventures Paintball Field</t>
@@ -512,7 +566,7 @@
     <t>Polk County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/off_the_wall_adventures/detail_page_images/OffWall/off-the-wall-paintball-logo-banner.jpg</t>
+    <t>https://paintballreservations.com/off_the_wall_adventures/detail_page_images/OffWall/off-the-wall-paintball-logo-banner.jpg</t>
   </si>
   <si>
     <t>Paintball and Airsoft Field</t>
@@ -527,7 +581,7 @@
     <t>Pierce County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/paintball_and_airsoft/detail_page_images/paintball-sports/Paintball-and-Airsoft.jpg</t>
+    <t>https://paintballreservations.com/paintball_and_airsoft/detail_page_images/paintball-sports/Paintball-and-Airsoft.jpg</t>
   </si>
   <si>
     <t>Paintball Bonanza Paintball Field</t>
@@ -539,7 +593,7 @@
     <t>Houston, TX  77085</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/paintball_bonanza/detail_page_images/paintball-bonanza/</t>
+    <t>https://paintballreservations.com/paintball_bonanza/detail_page_images/paintball-bonanza/</t>
   </si>
   <si>
     <t>Paintball Paradise Paintball Field</t>
@@ -554,7 +608,7 @@
     <t>Wise County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/paintball_paradise/detail_page_images/ParadisePB/</t>
+    <t>https://paintballreservations.com/paintball_paradise/detail_page_images/ParadisePB/</t>
   </si>
   <si>
     <t>Paintball Station Paintball Field</t>
@@ -581,7 +635,10 @@
     <t>Los Angeles County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/paintball_usa/detail_page_images/usa/</t>
+    <t>(661) 296-1416</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/paintball_usa/detail_page_images/usa/</t>
   </si>
   <si>
     <t>Paintball USA Paintball Park - Ventura</t>
@@ -608,12 +665,18 @@
     <t>Orting, WA  98360</t>
   </si>
   <si>
+    <t>(206) 673-4834</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/puyallup_paintball_field/detail_page_images/puyallup/PuyallupPaintballLogo.jpg</t>
   </si>
   <si>
     <t>Puyallup Zombie</t>
   </si>
   <si>
+    <t>(253) 656-6797</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/puyallup_zombie/detail_page_images/puyallup-zombie/</t>
   </si>
   <si>
@@ -635,10 +698,10 @@
     <t>Conley, GA  30288</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/safety_wolf_recreation/detail_page_images/SafetyWofl/safety-wolf-banner.jpg</t>
-  </si>
-  <si>
-    <t>http://paintballreservations.com/semper_fi_paintball/detail_page_images/semper/semper-fi-paintball-banner.jpg</t>
+    <t>https://paintballreservations.com/safety_wolf_recreation/detail_page_images/SafetyWofl/safety-wolf-banner.jpg</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/semper_fi_paintball/detail_page_images/semper/semper-fi-paintball-banner.jpg</t>
   </si>
   <si>
     <t>2480 Hwy 20</t>
@@ -650,13 +713,13 @@
     <t>Big Horn County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/shadow_walker_paintball/detail_page_images/ShadowWalker/shadow-walker-paintball-banner.jpg</t>
+    <t>https://paintballreservations.com/shadow_walker_paintball/detail_page_images/ShadowWalker/shadow-walker-paintball-banner.jpg</t>
   </si>
   <si>
     <t>17022 Burn Rd</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/skinny_joes_paintball/detail_page_images/Skinny/SJPBBanner.jpg</t>
+    <t>https://paintballreservations.com/skinny_joes_paintball/detail_page_images/Skinny/SJPBBanner.jpg</t>
   </si>
   <si>
     <t>Smokey Point Paintball</t>
@@ -665,7 +728,7 @@
     <t>16520 Smokey Point Blvd.</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/smokey_point_paintball/detail_page_images/smokey-point/Banner.jpg</t>
+    <t>https://paintballreservations.com/smokey_point_paintball/detail_page_images/smokey-point/Banner.jpg</t>
   </si>
   <si>
     <t>Southern Maryland Paintball</t>
@@ -683,7 +746,7 @@
   https://twitter.com/somdpaintball</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/southern_maryland_paintball/detail_page_images/southernmaryland/</t>
+    <t>https://paintballreservations.com/southern_maryland_paintball/detail_page_images/southernmaryland/</t>
   </si>
   <si>
     <t>Spent Paintball Field</t>
@@ -695,7 +758,7 @@
     <t>West Palm Beach, FL  33406</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/spent_paintball_field/detail_page_images/Spent/</t>
+    <t>https://paintballreservations.com/spent_paintball_field/detail_page_images/Spent/</t>
   </si>
   <si>
     <t>Splat Action Paintball Field</t>
@@ -710,7 +773,7 @@
     <t>Clackamas County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/splat_action_paintball/detail_page_images/Vida/splat-action-paintball-banner.jpg</t>
+    <t>https://paintballreservations.com/splat_action_paintball/detail_page_images/Vida/splat-action-paintball-banner.jpg</t>
   </si>
   <si>
     <t>1408 Lakeside Drive</t>
@@ -719,7 +782,7 @@
     <t>Brookshire, TX  77423</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/splatterhouse_paintball/detail_page_images/splatter-house/splatterhouse-banner.jpg</t>
+    <t>https://paintballreservations.com/splatterhouse_paintball/detail_page_images/splatter-house/splatterhouse-banner.jpg</t>
   </si>
   <si>
     <t>Survival Game Of Texas Paintball Field</t>
@@ -746,7 +809,7 @@
     <t>Harwood, TX  78632</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/tactical_paintball/detail_page_images/tactical-paintball/</t>
+    <t>https://paintballreservations.com/tactical_paintball/detail_page_images/tactical-paintball/</t>
   </si>
   <si>
     <t>2120 San Benito Street</t>
@@ -758,6 +821,9 @@
     <t>San Benito County</t>
   </si>
   <si>
+    <t>(831) 453-0421</t>
+  </si>
+  <si>
     <t>https://paintballreservations.com/tag_paintball/detail_page_images/tag/tag-paintball-banner.jpg</t>
   </si>
   <si>
@@ -773,7 +839,7 @@
     <t>Fort Bend County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/tanks_paintball/detail_page_images/tanks-paintball/</t>
+    <t>https://paintballreservations.com/tanks_paintball/detail_page_images/tanks-paintball/</t>
   </si>
   <si>
     <t>Urban War Zone Paintball Field</t>
@@ -785,7 +851,7 @@
     <t>Houston, TX  77023</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/urban_war_zone_paintball/detail_page_images/urban-war-zone/</t>
+    <t>https://paintballreservations.com/urban_war_zone_paintball/detail_page_images/urban-war-zone/</t>
   </si>
   <si>
     <t>Virtual Assault Paintball Field</t>
@@ -794,7 +860,7 @@
     <t>4103 East Mission Ave</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/virtual_assault_paintball/detail_page_images/VirtualAssault/virtual-assault-banner.jpg</t>
+    <t>https://paintballreservations.com/virtual_assault_paintball/detail_page_images/VirtualAssault/virtual-assault-banner.jpg</t>
   </si>
   <si>
     <t>3046 Portland Rd. NE</t>
@@ -806,7 +872,7 @@
     <t>Marion  County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/warpaint_indoor/detail_page_images/warpaint-indoor/</t>
+    <t>https://paintballreservations.com/warpaint_indoor/detail_page_images/warpaint-indoor/</t>
   </si>
   <si>
     <t>Warped Paintball Park (New!)</t>
@@ -818,7 +884,7 @@
     <t>Castaic, CA  91384</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/warped_paintball_park/detail_page_images/warped-paintball/Banner.jpg</t>
+    <t>https://paintballreservations.com/warped_paintball_park/detail_page_images/warped-paintball/Banner.jpg</t>
   </si>
   <si>
     <t>Woodinvile Indoor Paintball</t>
@@ -833,7 +899,7 @@
     <t>King County</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/woodinville_indoor_paintball/detail_page_images/woodinville-indoor/Woodinville-Paintball-logo-color-stacked.png</t>
+    <t>https://paintballreservations.com/woodinville_indoor_paintball/detail_page_images/woodinville-indoor/Woodinville-Paintball-logo-color-stacked.png</t>
   </si>
   <si>
     <t>Woods Creek Paintball Area</t>
@@ -842,7 +908,10 @@
     <t>6042 Woods Creek Rd</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/woods_creek_paintball_area/detail_page_images/WoodsCreek/</t>
+    <t>(425) 953-2773</t>
+  </si>
+  <si>
+    <t>https://paintballreservations.com/woods_creek_paintball_area/detail_page_images/WoodsCreek/</t>
   </si>
   <si>
     <t>XP Paintball Field</t>
@@ -854,7 +923,7 @@
     <t>Middleburg, FL  32068</t>
   </si>
   <si>
-    <t>http://paintballreservations.com/xp_paintball_field/detail_page_images/XPPaintball/</t>
+    <t>https://paintballreservations.com/xp_paintball_field/detail_page_images/XPPaintball/</t>
   </si>
 </sst>
 </file>
@@ -1318,8 +1387,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261c9d47-70ea-4de4-bd02-d0f7dc03df38}">
-  <dimension ref="A1:E67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{bd433587-e2b8-4446-b112-abdcd1bf5e05}">
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -1327,12 +1396,13 @@
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="29.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="118.857142857143" customWidth="1"/>
-    <col min="4" max="4" width="25.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="228.285714285714" customWidth="1"/>
+    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="119.857142857143" customWidth="1"/>
+    <col min="5" max="5" width="25.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="228.285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75">
+    <row r="1" spans="1:6" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1348,1031 +1418,1232 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="12.75">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="12.75">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="12.75">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.75">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12.75">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="12.75">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A27" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="12.75">
+      <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="12.75">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="12.75">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="12.75">
+      <c r="A34" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="12.75">
+      <c r="A36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="12.75">
+      <c r="A38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>183</v>
+      </c>
+      <c r="E38" t="s">
+        <v>181</v>
+      </c>
+      <c r="F38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A39" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="12.75">
+      <c r="A40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>192</v>
+      </c>
+      <c r="E40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A41" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="12.75">
+      <c r="A42" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" t="s">
+        <v>199</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42" t="s">
+        <v>200</v>
+      </c>
+      <c r="F42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A43" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="12.75">
+      <c r="A44" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" t="s">
+        <v>209</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>212</v>
+      </c>
+      <c r="E44" t="s">
+        <v>210</v>
+      </c>
+      <c r="F44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="12.75">
+      <c r="A45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.75">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.75">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="12.75">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.75">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="46" spans="1:6" ht="12.75">
+      <c r="A46" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" t="s">
+        <v>214</v>
+      </c>
+      <c r="C46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" t="s">
+        <v>220</v>
+      </c>
+      <c r="E46" t="s">
+        <v>215</v>
+      </c>
+      <c r="F46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A47" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75">
+      <c r="A48" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" t="s">
+        <v>226</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A49" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="12.75">
+      <c r="A50" t="s">
+        <v>229</v>
+      </c>
+      <c r="B50" t="s">
+        <v>230</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>232</v>
+      </c>
+      <c r="E50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" ht="12.75">
+      <c r="A51" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="12.75">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="12.75">
-      <c r="A20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.75">
-      <c r="A22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="12.75">
-      <c r="A24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="12.75">
-      <c r="A26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A27" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75">
-      <c r="A28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A29" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="12.75">
-      <c r="A30" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A31" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="12.75">
-      <c r="A32" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" t="s">
-        <v>138</v>
-      </c>
-      <c r="D32" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="12.75">
-      <c r="A34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A35" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="12.75">
-      <c r="A36" t="s">
-        <v>151</v>
-      </c>
-      <c r="B36" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" t="s">
-        <v>155</v>
-      </c>
-      <c r="D36" t="s">
-        <v>153</v>
-      </c>
-      <c r="E36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A37" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="12.75">
-      <c r="A38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B38" t="s">
-        <v>162</v>
-      </c>
-      <c r="C38" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A39" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="12.75">
-      <c r="A40" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A41" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="12.75">
-      <c r="A42" t="s">
-        <v>180</v>
-      </c>
-      <c r="B42" t="s">
-        <v>181</v>
-      </c>
-      <c r="C42" t="s">
-        <v>183</v>
-      </c>
-      <c r="D42" t="s">
-        <v>182</v>
-      </c>
-      <c r="E42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A43" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="12.75">
-      <c r="A44" t="s">
-        <v>189</v>
-      </c>
-      <c r="B44" t="s">
-        <v>190</v>
-      </c>
-      <c r="C44" t="s">
-        <v>193</v>
-      </c>
-      <c r="D44" t="s">
-        <v>191</v>
-      </c>
-      <c r="E44" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" ht="12.75">
-      <c r="A45" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="12.75">
-      <c r="A46" t="s">
-        <v>198</v>
-      </c>
-      <c r="B46" t="s">
-        <v>195</v>
-      </c>
-      <c r="C46" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" t="s">
-        <v>196</v>
-      </c>
-      <c r="E46" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A47" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="12.75">
-      <c r="A48" t="s">
-        <v>204</v>
-      </c>
-      <c r="B48" t="s">
-        <v>205</v>
-      </c>
-      <c r="C48" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="12.75">
-      <c r="A50" t="s">
-        <v>208</v>
-      </c>
-      <c r="B50" t="s">
-        <v>209</v>
-      </c>
-      <c r="C50" t="s">
-        <v>211</v>
-      </c>
-      <c r="D50" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="2" customFormat="1" ht="12.75">
-      <c r="A51" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="12.75">
+    </row>
+    <row r="52" spans="1:6" ht="12.75">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
       <c r="C52" t="s">
         <v>216</v>
       </c>
       <c r="D52" t="s">
-        <v>146</v>
+        <v>237</v>
       </c>
       <c r="E52" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" ht="12.75">
+        <v>160</v>
+      </c>
+      <c r="F52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A53" s="2" t="s">
-        <v>217</v>
+        <v>238</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>221</v>
+        <v>8</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="12.75">
+        <v>240</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="12.75">
       <c r="A54" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="B54" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="C54" t="s">
-        <v>225</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" ht="12.75">
+        <v>246</v>
+      </c>
+      <c r="E54" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A55" s="2" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>230</v>
+        <v>8</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="12.75">
+        <v>249</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="12.75">
       <c r="A56" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="B56" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="C56" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="2" customFormat="1" ht="12.75">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A57" s="2" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>238</v>
+        <v>8</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="12.75">
+        <v>257</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="12.75">
       <c r="A58" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="B58" t="s">
-        <v>240</v>
+        <v>261</v>
       </c>
       <c r="C58" t="s">
-        <v>242</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>263</v>
+      </c>
+      <c r="E58" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A59" s="2" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="12.75">
+        <v>268</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="12.75">
       <c r="A60" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="B60" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="C60" t="s">
-        <v>251</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="E60" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>271</v>
+      </c>
+      <c r="F60" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A61" s="2" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="12.75">
+        <v>277</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="12.75">
       <c r="A62" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="B62" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="C62" t="s">
-        <v>258</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>280</v>
       </c>
       <c r="E62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>11</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A63" s="2" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>262</v>
+        <v>8</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="12.75">
+        <v>284</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="12.75">
       <c r="A64" t="s">
-        <v>263</v>
+        <v>285</v>
       </c>
       <c r="B64" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="C64" t="s">
-        <v>266</v>
+        <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="E64" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="2" customFormat="1" ht="12.75">
+        <v>287</v>
+      </c>
+      <c r="F64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="2" customFormat="1" ht="12.75">
       <c r="A65" s="2" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>271</v>
+        <v>8</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="12.75">
+        <v>291</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="12.75">
       <c r="A66" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="B66" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="C66" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="D66" t="s">
-        <v>60</v>
+        <v>297</v>
       </c>
       <c r="E66" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" s="2" customFormat="1" ht="12.75">
+        <v>66</v>
+      </c>
+      <c r="F66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="2" customFormat="1" ht="12.75">
       <c r="A67" s="2" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>278</v>
+        <v>8</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>277</v>
+        <v>301</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>